<commit_message>
Meetrapport klaar voor puntjes op de I
</commit_message>
<xml_diff>
--- a/testsets/Set B Saturation/Metingen Saturation/Diagrammen Saturation.xlsx
+++ b/testsets/Set B Saturation/Metingen Saturation/Diagrammen Saturation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ties1\OneDrive\Bureaublad\STUDIE\HBO-ICT jaar 2019-2020\Vision\Github repo\HU-Vision-Ties-Mick\testsets\Set B Saturation\Metingen Saturation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mickb\source\repos\Tiesbrouwer10\HU-Vision-Ties-Mick\testsets\Set B Saturation\Metingen Saturation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92E1233-9717-4E83-8048-435CD90C48A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEC4BD9-BC21-483B-8419-13DA1EE0BC27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-8835" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -109,7 +109,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1100,7 +1100,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2095,7 +2095,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3090,7 +3090,7 @@
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4085,7 +4085,7 @@
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5079,7 +5079,7 @@
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6073,7 +6073,7 @@
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7069,7 +7069,7 @@
 <file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8064,7 +8064,7 @@
 <file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -9059,7 +9059,7 @@
 <file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -10053,7 +10053,7 @@
 <file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -11047,7 +11047,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -12041,7 +12041,7 @@
 <file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -13036,7 +13036,7 @@
 <file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -14031,7 +14031,7 @@
 <file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -15026,7 +15026,7 @@
 <file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -16020,7 +16020,7 @@
 <file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -17014,7 +17014,7 @@
 <file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -18020,7 +18020,7 @@
 <file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -19015,7 +19015,7 @@
 <file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -20010,7 +20010,7 @@
 <file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -21004,7 +21004,7 @@
 <file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -21998,7 +21998,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -22992,7 +22992,7 @@
 <file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -23998,7 +23998,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -24992,7 +24992,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -25986,7 +25986,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -26984,7 +26984,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -27982,7 +27982,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -28979,7 +28979,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -59403,7 +59403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B9:B97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>